<commit_message>
Lan thu hai da them vao 2/1/2018
</commit_message>
<xml_diff>
--- a/danhsach_hangHoa.xlsx
+++ b/danhsach_hangHoa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Chau</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>1 tỉ</t>
+  </si>
+  <si>
+    <t>2/1/2/108</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,6 +394,14 @@
         <v>43101</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vừa mới chi 4 tỉ
</commit_message>
<xml_diff>
--- a/danhsach_hangHoa.xlsx
+++ b/danhsach_hangHoa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Chau</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>3 tỉ</t>
+  </si>
+  <si>
+    <t>4 tỉ</t>
   </si>
 </sst>
 </file>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,6 +414,11 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>